<commit_message>
Adding Item Objects and updated room assignments excel
</commit_message>
<xml_diff>
--- a/room_assignments.xlsx
+++ b/room_assignments.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17927"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
   <si>
     <t>Room</t>
   </si>
@@ -82,6 +82,36 @@
   </si>
   <si>
     <t>Brent</t>
+  </si>
+  <si>
+    <t>Items</t>
+  </si>
+  <si>
+    <t>button</t>
+  </si>
+  <si>
+    <t>blaster pistol</t>
+  </si>
+  <si>
+    <t>model sailing ship</t>
+  </si>
+  <si>
+    <t>plastic pass key</t>
+  </si>
+  <si>
+    <t>hibernation pod</t>
+  </si>
+  <si>
+    <t>blue rose</t>
+  </si>
+  <si>
+    <t>android</t>
+  </si>
+  <si>
+    <t>reactor fuel</t>
+  </si>
+  <si>
+    <t>Features (must have two)</t>
   </si>
 </sst>
 </file>
@@ -408,151 +438,182 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" customWidth="1"/>
+    <col min="1" max="1" width="17.5546875" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>8</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>13</v>
       </c>
       <c r="B12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>15</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B24" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>16</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B26" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="C26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>17</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B28" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="C28" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>18</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B30" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="C30" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>19</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B32" t="s">
         <v>20</v>
+      </c>
+      <c r="C32" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
small excel sheet change
</commit_message>
<xml_diff>
--- a/room_assignments.xlsx
+++ b/room_assignments.xlsx
@@ -440,14 +440,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.5546875" customWidth="1"/>
     <col min="3" max="3" width="14.6640625" customWidth="1"/>
+    <col min="4" max="4" width="28.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Adding new features and updating room assignment legend
</commit_message>
<xml_diff>
--- a/room_assignments.xlsx
+++ b/room_assignments.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="51">
   <si>
     <t>Room</t>
   </si>
@@ -30,9 +30,6 @@
     <t>Bridge</t>
   </si>
   <si>
-    <t>Elevator</t>
-  </si>
-  <si>
     <t>Crew Quarters</t>
   </si>
   <si>
@@ -112,6 +109,69 @@
   </si>
   <si>
     <t>Features (must have two)</t>
+  </si>
+  <si>
+    <t>crops</t>
+  </si>
+  <si>
+    <t>turtle</t>
+  </si>
+  <si>
+    <t>manifest</t>
+  </si>
+  <si>
+    <t>packages</t>
+  </si>
+  <si>
+    <t>leftovers</t>
+  </si>
+  <si>
+    <t>dying man</t>
+  </si>
+  <si>
+    <t>dying alien</t>
+  </si>
+  <si>
+    <t>alien notes</t>
+  </si>
+  <si>
+    <t>table of notes</t>
+  </si>
+  <si>
+    <t>telescope</t>
+  </si>
+  <si>
+    <t>pistol instructions</t>
+  </si>
+  <si>
+    <t>bow</t>
+  </si>
+  <si>
+    <t>window</t>
+  </si>
+  <si>
+    <t>notepad</t>
+  </si>
+  <si>
+    <t>diary</t>
+  </si>
+  <si>
+    <t>Elevator 1</t>
+  </si>
+  <si>
+    <t>Elevator 2</t>
+  </si>
+  <si>
+    <t>Elevator 3</t>
+  </si>
+  <si>
+    <t>map</t>
+  </si>
+  <si>
+    <t>speaker</t>
+  </si>
+  <si>
+    <t>pajamas</t>
   </si>
 </sst>
 </file>
@@ -438,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -459,10 +519,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -470,151 +530,255 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D5" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>46</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
-        <v>7</v>
+      <c r="D8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D9" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" t="s">
-        <v>24</v>
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D11" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>10</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B22" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" t="s">
+        <v>22</v>
+      </c>
+      <c r="D26" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D27" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>11</v>
-      </c>
-      <c r="B18" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>12</v>
-      </c>
-      <c r="B20" t="s">
-        <v>14</v>
-      </c>
-      <c r="C20" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>13</v>
-      </c>
-      <c r="B22" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="B28" t="s">
+        <v>19</v>
+      </c>
+      <c r="D28" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D29" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>15</v>
       </c>
-      <c r="B24" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>16</v>
-      </c>
-      <c r="B26" t="s">
-        <v>20</v>
-      </c>
-      <c r="C26" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>17</v>
-      </c>
-      <c r="B28" t="s">
-        <v>20</v>
-      </c>
-      <c r="C28" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>18</v>
-      </c>
       <c r="B30" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C30" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D30" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D31" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
+        <v>16</v>
+      </c>
+      <c r="B32" t="s">
         <v>19</v>
       </c>
-      <c r="B32" t="s">
-        <v>20</v>
-      </c>
       <c r="C32" t="s">
+        <v>24</v>
+      </c>
+      <c r="D32" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D33" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>17</v>
+      </c>
+      <c r="B34" t="s">
+        <v>19</v>
+      </c>
+      <c r="C34" t="s">
         <v>26</v>
+      </c>
+      <c r="D34" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D35" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>18</v>
+      </c>
+      <c r="B36" t="s">
+        <v>19</v>
+      </c>
+      <c r="C36" t="s">
+        <v>25</v>
+      </c>
+      <c r="D36" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D37" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>